<commit_message>
change in brand entry N.A change
</commit_message>
<xml_diff>
--- a/public/excel/BrandDetails.xlsx
+++ b/public/excel/BrandDetails.xlsx
@@ -47,7 +47,7 @@
     <t>WhatsApp</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Not Applicable</t>
   </si>
   <si>
     <t>Y</t>
@@ -56,7 +56,7 @@
     <t>Facebook</t>
   </si>
   <si>
-    <t>https://www.facebook.com</t>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -398,18 +398,18 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F1" sqref="F1:F4"/>
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="15" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="15" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -482,7 +482,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -492,6 +492,26 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12546636</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>